<commit_message>
change data format to csv
</commit_message>
<xml_diff>
--- a/FPS_DATA.xlsx
+++ b/FPS_DATA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\FPSCrawl\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\fpsPrediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97FFEB4B-0375-47E6-B3B3-73CED19C80B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B26E4F-7413-4E40-8E00-3D8D2573B033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{41DB647D-F351-4E6D-ACAF-B2E7CC4F09D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{41DB647D-F351-4E6D-ACAF-B2E7CC4F09D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -246,9 +246,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PlayerUnknown's Battlegrounds</t>
-  </si>
-  <si>
     <t>Intel Core i5-6600K 3.5GHz</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -271,6 +268,10 @@
   </si>
   <si>
     <t>Game#</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PlayerUnknown's Battlegrounds</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -647,12 +648,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36B4FA40-62D6-4DFA-9D99-B78AD52D3373}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:R331"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O11" sqref="O11"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -6781,7 +6781,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>11</v>
       </c>
@@ -6837,7 +6837,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="111" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>11</v>
       </c>
@@ -6893,7 +6893,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="112" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>11</v>
       </c>
@@ -6949,7 +6949,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="113" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>11</v>
       </c>
@@ -7005,7 +7005,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="114" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>11</v>
       </c>
@@ -7061,7 +7061,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="115" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>11</v>
       </c>
@@ -7117,7 +7117,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="116" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>11</v>
       </c>
@@ -7173,7 +7173,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="117" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>11</v>
       </c>
@@ -7229,7 +7229,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="118" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>11</v>
       </c>
@@ -7285,7 +7285,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="119" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>11</v>
       </c>
@@ -7341,7 +7341,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="120" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>11</v>
       </c>
@@ -7397,7 +7397,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="121" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>11</v>
       </c>
@@ -7453,7 +7453,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="122" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>11</v>
       </c>
@@ -7509,7 +7509,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="123" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>11</v>
       </c>
@@ -7565,7 +7565,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="124" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>11</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="125" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>11</v>
       </c>
@@ -7677,7 +7677,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="126" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>11</v>
       </c>
@@ -7733,7 +7733,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="127" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>11</v>
       </c>
@@ -7789,7 +7789,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="128" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>11</v>
       </c>
@@ -7845,7 +7845,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="129" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>11</v>
       </c>
@@ -7901,7 +7901,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="130" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>11</v>
       </c>
@@ -7957,7 +7957,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="131" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>11</v>
       </c>
@@ -8013,7 +8013,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="132" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>11</v>
       </c>
@@ -8069,7 +8069,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="133" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>11</v>
       </c>
@@ -8125,7 +8125,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="134" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>11</v>
       </c>
@@ -8181,7 +8181,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="135" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>11</v>
       </c>
@@ -8237,7 +8237,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="136" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>11</v>
       </c>
@@ -8293,7 +8293,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="137" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>11</v>
       </c>
@@ -8349,7 +8349,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="138" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>11</v>
       </c>
@@ -8405,7 +8405,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="139" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>11</v>
       </c>
@@ -8461,7 +8461,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="140" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>11</v>
       </c>
@@ -8517,7 +8517,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="141" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>11</v>
       </c>
@@ -8573,7 +8573,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="142" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>11</v>
       </c>
@@ -8629,7 +8629,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="143" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>11</v>
       </c>
@@ -8685,7 +8685,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="144" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>11</v>
       </c>
@@ -8741,7 +8741,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="145" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>11</v>
       </c>
@@ -8797,7 +8797,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="146" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>11</v>
       </c>
@@ -8853,7 +8853,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="147" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>11</v>
       </c>
@@ -8909,7 +8909,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="148" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>11</v>
       </c>
@@ -8965,7 +8965,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="149" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>11</v>
       </c>
@@ -9021,7 +9021,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="150" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>11</v>
       </c>
@@ -9077,7 +9077,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="151" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>11</v>
       </c>
@@ -9133,7 +9133,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="152" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>11</v>
       </c>
@@ -9189,7 +9189,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="153" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>11</v>
       </c>
@@ -9245,7 +9245,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="154" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>11</v>
       </c>
@@ -9301,7 +9301,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="155" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>11</v>
       </c>
@@ -9357,7 +9357,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="156" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>11</v>
       </c>
@@ -9413,7 +9413,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="157" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>11</v>
       </c>
@@ -9469,7 +9469,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="158" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>11</v>
       </c>
@@ -9525,7 +9525,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="159" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>11</v>
       </c>
@@ -9581,7 +9581,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="160" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>11</v>
       </c>
@@ -9637,7 +9637,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="161" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>32</v>
       </c>
@@ -9693,7 +9693,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="162" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>32</v>
       </c>
@@ -9749,7 +9749,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="163" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>32</v>
       </c>
@@ -9805,7 +9805,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="164" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>32</v>
       </c>
@@ -9861,7 +9861,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="165" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>32</v>
       </c>
@@ -9917,7 +9917,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="166" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>32</v>
       </c>
@@ -9973,7 +9973,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="167" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>32</v>
       </c>
@@ -10029,7 +10029,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="168" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>32</v>
       </c>
@@ -10085,7 +10085,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="169" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>32</v>
       </c>
@@ -10141,7 +10141,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="170" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>32</v>
       </c>
@@ -10197,7 +10197,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="171" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>32</v>
       </c>
@@ -10253,7 +10253,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="172" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>32</v>
       </c>
@@ -10309,7 +10309,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="173" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>32</v>
       </c>
@@ -10365,7 +10365,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="174" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>32</v>
       </c>
@@ -10421,7 +10421,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="175" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>32</v>
       </c>
@@ -10477,7 +10477,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="176" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>32</v>
       </c>
@@ -10533,7 +10533,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="177" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>32</v>
       </c>
@@ -10589,7 +10589,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="178" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
         <v>32</v>
       </c>
@@ -10645,7 +10645,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="179" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
         <v>32</v>
       </c>
@@ -10701,7 +10701,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="180" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
         <v>32</v>
       </c>
@@ -10757,7 +10757,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="181" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
         <v>32</v>
       </c>
@@ -10813,7 +10813,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="182" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
         <v>32</v>
       </c>
@@ -10869,7 +10869,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="183" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
         <v>32</v>
       </c>
@@ -10925,7 +10925,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="184" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
         <v>32</v>
       </c>
@@ -10981,7 +10981,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="185" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
         <v>32</v>
       </c>
@@ -11037,7 +11037,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="186" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
         <v>32</v>
       </c>
@@ -11093,7 +11093,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="187" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
         <v>32</v>
       </c>
@@ -11149,7 +11149,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="188" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
         <v>32</v>
       </c>
@@ -11205,7 +11205,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="189" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
         <v>32</v>
       </c>
@@ -11261,7 +11261,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="190" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
         <v>32</v>
       </c>
@@ -11317,7 +11317,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="191" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
         <v>32</v>
       </c>
@@ -11373,7 +11373,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="192" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
         <v>32</v>
       </c>
@@ -11429,7 +11429,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="193" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
         <v>32</v>
       </c>
@@ -11485,7 +11485,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="194" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
         <v>32</v>
       </c>
@@ -11541,7 +11541,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="195" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
         <v>32</v>
       </c>
@@ -11597,7 +11597,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="196" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
         <v>32</v>
       </c>
@@ -11653,7 +11653,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="197" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
         <v>32</v>
       </c>
@@ -11709,7 +11709,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="198" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
         <v>32</v>
       </c>
@@ -11765,7 +11765,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="199" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
         <v>32</v>
       </c>
@@ -11821,7 +11821,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="200" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
         <v>32</v>
       </c>
@@ -11877,7 +11877,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="201" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
         <v>32</v>
       </c>
@@ -11933,7 +11933,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="202" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
         <v>32</v>
       </c>
@@ -11989,7 +11989,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="203" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
         <v>32</v>
       </c>
@@ -12045,7 +12045,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="204" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A204" t="s">
         <v>32</v>
       </c>
@@ -12101,7 +12101,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="205" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
         <v>32</v>
       </c>
@@ -12157,7 +12157,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="206" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
         <v>32</v>
       </c>
@@ -12213,7 +12213,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="207" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
         <v>32</v>
       </c>
@@ -12269,7 +12269,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="208" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
         <v>32</v>
       </c>
@@ -12325,7 +12325,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="209" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
         <v>42</v>
       </c>
@@ -12381,7 +12381,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="210" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
         <v>42</v>
       </c>
@@ -12437,7 +12437,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="211" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
         <v>42</v>
       </c>
@@ -12493,7 +12493,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="212" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
         <v>42</v>
       </c>
@@ -12549,7 +12549,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="213" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
         <v>42</v>
       </c>
@@ -12605,7 +12605,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="214" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
         <v>42</v>
       </c>
@@ -12661,7 +12661,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="215" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
         <v>42</v>
       </c>
@@ -12717,7 +12717,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="216" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
         <v>42</v>
       </c>
@@ -12773,7 +12773,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="217" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
         <v>42</v>
       </c>
@@ -12829,12 +12829,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="218" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
         <v>42</v>
       </c>
       <c r="B218" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C218">
         <v>19830</v>
@@ -12852,7 +12852,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H218" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I218">
         <v>2561</v>
@@ -12885,12 +12885,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="219" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
         <v>42</v>
       </c>
       <c r="B219" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C219">
         <v>19830</v>
@@ -12908,7 +12908,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H219" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I219">
         <v>2561</v>
@@ -12941,12 +12941,12 @@
         <v>30</v>
       </c>
     </row>
-    <row r="220" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
         <v>42</v>
       </c>
       <c r="B220" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C220">
         <v>19830</v>
@@ -12964,7 +12964,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H220" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I220">
         <v>2561</v>
@@ -12997,7 +12997,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="221" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
         <v>11</v>
       </c>
@@ -13053,7 +13053,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="222" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
         <v>11</v>
       </c>
@@ -13109,7 +13109,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="223" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
         <v>11</v>
       </c>
@@ -13165,7 +13165,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="224" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
         <v>11</v>
       </c>
@@ -13221,7 +13221,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="225" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
         <v>11</v>
       </c>
@@ -13277,7 +13277,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="226" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
         <v>11</v>
       </c>
@@ -13333,7 +13333,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="227" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
         <v>11</v>
       </c>
@@ -13389,7 +13389,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="228" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
         <v>11</v>
       </c>
@@ -13445,7 +13445,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="229" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
         <v>11</v>
       </c>
@@ -13501,7 +13501,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="230" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
         <v>11</v>
       </c>
@@ -13557,7 +13557,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="231" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
         <v>11</v>
       </c>
@@ -13613,7 +13613,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="232" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
         <v>11</v>
       </c>
@@ -13669,7 +13669,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="233" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
         <v>11</v>
       </c>
@@ -13725,7 +13725,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="234" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
         <v>11</v>
       </c>
@@ -13781,7 +13781,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="235" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
         <v>11</v>
       </c>
@@ -13837,7 +13837,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="236" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
         <v>11</v>
       </c>
@@ -13893,7 +13893,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="237" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
         <v>11</v>
       </c>
@@ -13949,7 +13949,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="238" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
         <v>11</v>
       </c>
@@ -14005,7 +14005,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="239" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
         <v>11</v>
       </c>
@@ -14061,7 +14061,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="240" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
         <v>11</v>
       </c>
@@ -14117,7 +14117,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="241" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
         <v>11</v>
       </c>
@@ -14173,7 +14173,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="242" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
         <v>11</v>
       </c>
@@ -14229,7 +14229,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="243" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
         <v>11</v>
       </c>
@@ -14285,7 +14285,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="244" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
         <v>11</v>
       </c>
@@ -14341,7 +14341,7 @@
         <v>1100</v>
       </c>
     </row>
-    <row r="245" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
         <v>11</v>
       </c>
@@ -14397,7 +14397,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="246" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
         <v>11</v>
       </c>
@@ -14453,7 +14453,7 @@
         <v>840</v>
       </c>
     </row>
-    <row r="247" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
         <v>11</v>
       </c>
@@ -14509,7 +14509,7 @@
         <v>1096</v>
       </c>
     </row>
-    <row r="248" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
         <v>11</v>
       </c>
@@ -14565,7 +14565,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="249" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
         <v>11</v>
       </c>
@@ -14621,7 +14621,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="250" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
         <v>11</v>
       </c>
@@ -14677,7 +14677,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="251" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
         <v>11</v>
       </c>
@@ -14733,7 +14733,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="252" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
         <v>11</v>
       </c>
@@ -14789,7 +14789,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="253" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
         <v>11</v>
       </c>
@@ -14845,7 +14845,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="254" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
         <v>11</v>
       </c>
@@ -14901,7 +14901,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="255" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
         <v>11</v>
       </c>
@@ -14957,7 +14957,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="256" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
         <v>11</v>
       </c>
@@ -15013,7 +15013,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="257" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
         <v>11</v>
       </c>
@@ -15069,7 +15069,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="258" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
         <v>11</v>
       </c>
@@ -15125,7 +15125,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="259" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
         <v>11</v>
       </c>
@@ -15181,7 +15181,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="260" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
         <v>11</v>
       </c>
@@ -15237,7 +15237,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="261" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
         <v>11</v>
       </c>
@@ -15293,7 +15293,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="262" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
         <v>11</v>
       </c>
@@ -15349,7 +15349,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="263" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
         <v>11</v>
       </c>
@@ -15405,7 +15405,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="264" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
         <v>11</v>
       </c>
@@ -15461,7 +15461,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="265" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
         <v>11</v>
       </c>
@@ -15517,7 +15517,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="266" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
         <v>11</v>
       </c>
@@ -15573,7 +15573,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="267" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
         <v>11</v>
       </c>
@@ -15629,7 +15629,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="268" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
         <v>11</v>
       </c>
@@ -15685,7 +15685,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="269" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
         <v>11</v>
       </c>
@@ -15741,7 +15741,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="270" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
         <v>11</v>
       </c>
@@ -15797,7 +15797,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="271" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
         <v>11</v>
       </c>
@@ -15853,7 +15853,7 @@
         <v>1040</v>
       </c>
     </row>
-    <row r="272" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
         <v>32</v>
       </c>
@@ -15909,7 +15909,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="273" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
         <v>32</v>
       </c>
@@ -15965,7 +15965,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="274" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
         <v>32</v>
       </c>
@@ -16021,7 +16021,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="275" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
         <v>32</v>
       </c>
@@ -16077,7 +16077,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="276" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
         <v>32</v>
       </c>
@@ -16133,7 +16133,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="277" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
         <v>32</v>
       </c>
@@ -16189,7 +16189,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="278" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
         <v>32</v>
       </c>
@@ -16245,7 +16245,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="279" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
         <v>32</v>
       </c>
@@ -16301,7 +16301,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="280" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
         <v>32</v>
       </c>
@@ -16357,7 +16357,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="281" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
         <v>32</v>
       </c>
@@ -16413,7 +16413,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="282" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
         <v>32</v>
       </c>
@@ -16469,7 +16469,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="283" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
         <v>32</v>
       </c>
@@ -16525,7 +16525,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="284" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
         <v>32</v>
       </c>
@@ -16581,7 +16581,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="285" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A285" t="s">
         <v>32</v>
       </c>
@@ -16637,7 +16637,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="286" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A286" t="s">
         <v>32</v>
       </c>
@@ -16693,7 +16693,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="287" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A287" t="s">
         <v>32</v>
       </c>
@@ -16749,7 +16749,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="288" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A288" t="s">
         <v>32</v>
       </c>
@@ -16805,7 +16805,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="289" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A289" t="s">
         <v>32</v>
       </c>
@@ -16861,7 +16861,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="290" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A290" t="s">
         <v>32</v>
       </c>
@@ -16917,7 +16917,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="291" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A291" t="s">
         <v>32</v>
       </c>
@@ -16973,7 +16973,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="292" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A292" t="s">
         <v>32</v>
       </c>
@@ -17029,7 +17029,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="293" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A293" t="s">
         <v>32</v>
       </c>
@@ -17085,7 +17085,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="294" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A294" t="s">
         <v>32</v>
       </c>
@@ -17141,7 +17141,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="295" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A295" t="s">
         <v>32</v>
       </c>
@@ -17197,7 +17197,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="296" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A296" t="s">
         <v>32</v>
       </c>
@@ -17253,7 +17253,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="297" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A297" t="s">
         <v>32</v>
       </c>
@@ -17309,7 +17309,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="298" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A298" t="s">
         <v>32</v>
       </c>
@@ -17365,7 +17365,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="299" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A299" t="s">
         <v>32</v>
       </c>
@@ -17421,7 +17421,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="300" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A300" t="s">
         <v>32</v>
       </c>
@@ -17477,7 +17477,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="301" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A301" t="s">
         <v>32</v>
       </c>
@@ -17533,7 +17533,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="302" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A302" t="s">
         <v>32</v>
       </c>
@@ -17589,7 +17589,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="303" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A303" t="s">
         <v>32</v>
       </c>
@@ -17645,7 +17645,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="304" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A304" t="s">
         <v>32</v>
       </c>
@@ -17701,7 +17701,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="305" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A305" t="s">
         <v>32</v>
       </c>
@@ -17757,7 +17757,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="306" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A306" t="s">
         <v>32</v>
       </c>
@@ -17813,7 +17813,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="307" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A307" t="s">
         <v>32</v>
       </c>
@@ -17869,7 +17869,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="308" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
         <v>32</v>
       </c>
@@ -17925,7 +17925,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="309" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A309" t="s">
         <v>32</v>
       </c>
@@ -17981,7 +17981,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="310" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A310" t="s">
         <v>32</v>
       </c>
@@ -18037,7 +18037,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="311" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A311" t="s">
         <v>32</v>
       </c>
@@ -18093,7 +18093,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="312" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A312" t="s">
         <v>32</v>
       </c>
@@ -18149,7 +18149,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="313" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A313" t="s">
         <v>32</v>
       </c>
@@ -18205,7 +18205,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="314" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A314" t="s">
         <v>32</v>
       </c>
@@ -18261,7 +18261,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="315" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A315" t="s">
         <v>32</v>
       </c>
@@ -18317,7 +18317,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="316" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A316" t="s">
         <v>32</v>
       </c>
@@ -18373,7 +18373,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="317" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A317" t="s">
         <v>32</v>
       </c>
@@ -18429,7 +18429,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="318" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A318" t="s">
         <v>32</v>
       </c>
@@ -18485,7 +18485,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="319" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
         <v>32</v>
       </c>
@@ -18541,7 +18541,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="320" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
         <v>42</v>
       </c>
@@ -18597,7 +18597,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="321" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A321" t="s">
         <v>42</v>
       </c>
@@ -18653,7 +18653,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="322" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
         <v>42</v>
       </c>
@@ -18709,7 +18709,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="323" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A323" t="s">
         <v>42</v>
       </c>
@@ -18765,7 +18765,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="324" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A324" t="s">
         <v>42</v>
       </c>
@@ -18821,7 +18821,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="325" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
         <v>42</v>
       </c>
@@ -18877,7 +18877,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="326" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A326" t="s">
         <v>42</v>
       </c>
@@ -18933,7 +18933,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="327" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A327" t="s">
         <v>42</v>
       </c>
@@ -18989,7 +18989,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="328" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A328" t="s">
         <v>42</v>
       </c>
@@ -19045,12 +19045,12 @@
         <v>210</v>
       </c>
     </row>
-    <row r="329" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A329" t="s">
         <v>42</v>
       </c>
       <c r="B329" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C329">
         <v>19830</v>
@@ -19068,7 +19068,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H329" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I329">
         <v>2561</v>
@@ -19101,12 +19101,12 @@
         <v>150</v>
       </c>
     </row>
-    <row r="330" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A330" t="s">
         <v>42</v>
       </c>
       <c r="B330" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C330">
         <v>19830</v>
@@ -19124,7 +19124,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H330" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I330">
         <v>2561</v>
@@ -19157,12 +19157,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="331" spans="1:18" hidden="1" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A331" t="s">
         <v>42</v>
       </c>
       <c r="B331" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C331">
         <v>19830</v>
@@ -19180,7 +19180,7 @@
         <v>4.4000000000000004</v>
       </c>
       <c r="H331" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I331">
         <v>2561</v>
@@ -19214,13 +19214,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:R331" xr:uid="{36B4FA40-62D6-4DFA-9D99-B78AD52D3373}">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="1"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B1:R331" xr:uid="{36B4FA40-62D6-4DFA-9D99-B78AD52D3373}"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="H2" r:id="rId1" display="https://www.techpowerup.com/gpu-specs/geforce-rtx-3090-ti.c3829" xr:uid="{A132A7AB-944D-438F-B519-2D114EF4199D}"/>
@@ -19261,7 +19255,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -19273,7 +19267,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B1" t="s">
         <v>6</v>
@@ -19304,10 +19298,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" t="s">
         <v>53</v>
-      </c>
-      <c r="C3" t="s">
-        <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>29</v>
@@ -19318,13 +19312,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
         <v>57</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>58</v>
-      </c>
-      <c r="D4" t="s">
-        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit kfold + linear regression
</commit_message>
<xml_diff>
--- a/FPS_DATA.xlsx
+++ b/FPS_DATA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\fpsPrediction\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B26E4F-7413-4E40-8E00-3D8D2573B033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4A34A59-B0CC-4D62-A9D1-C26EB954C170}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{41DB647D-F351-4E6D-ACAF-B2E7CC4F09D3}"/>
   </bookViews>
@@ -651,8 +651,8 @@
   <dimension ref="A1:R331"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
+      <pane ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L224" sqref="L224"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>